<commit_message>
Add ID to Albuwell sample sheet
</commit_message>
<xml_diff>
--- a/VQC R work/Albuwell Data Sheets/Long_PFAS_Albuwell_Sample_061225.xlsx
+++ b/VQC R work/Albuwell Data Sheets/Long_PFAS_Albuwell_Sample_061225.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://keckmedicine-my.sharepoint.com/personal/victoria_quonchow_med_usc_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriaqc/Documents/GitHub/PFAS_met_cage/VQC R work/Albuwell Data Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A390410B-EECE-E14E-B5C2-076A6D6FDCEB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CF3390-F890-1845-BDCD-E9B1BEF771B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2100" windowWidth="18060" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2100" windowWidth="28220" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="129">
   <si>
     <t>Cell</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>3939_Final</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -808,19 +811,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O97"/>
+  <dimension ref="A1:P97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88:E93"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -831,16 +834,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -853,8 +859,9 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -863,8 +870,9 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -874,15 +882,18 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1">
-        <v>10</v>
-      </c>
+      <c r="D4" s="1">
+        <v>3920</v>
+      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -892,15 +903,18 @@
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1">
-        <v>10</v>
-      </c>
+      <c r="D5" s="1">
+        <v>3920</v>
+      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -910,15 +924,18 @@
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
-        <v>10</v>
-      </c>
+      <c r="D6" s="1">
+        <v>3932</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -928,15 +945,18 @@
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1">
-        <v>10</v>
-      </c>
+      <c r="D7" s="1">
+        <v>3932</v>
+      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -946,15 +966,18 @@
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
+      <c r="D8" s="1">
+        <v>3936</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
         <v>5</v>
       </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -964,15 +987,18 @@
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
+      <c r="D9" s="1">
+        <v>3936</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
         <v>5</v>
       </c>
-      <c r="F9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -981,8 +1007,9 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -991,17 +1018,18 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="M11" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G11" s="1"/>
       <c r="N11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1010,17 +1038,18 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="M12" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="N12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1029,17 +1058,18 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="M13" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G13" s="1"/>
       <c r="N13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1">
+        <v>10</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="1">
         <v>1.25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1049,18 +1079,19 @@
       <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="1">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="M14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1070,18 +1101,19 @@
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1">
-        <v>10</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="M15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1091,18 +1123,21 @@
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1">
-        <v>10</v>
-      </c>
+      <c r="D16" s="1">
+        <v>3920</v>
+      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="M16" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1112,18 +1147,21 @@
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1">
-        <v>10</v>
-      </c>
+      <c r="D17" s="1">
+        <v>3920</v>
+      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="M17" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1133,18 +1171,21 @@
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1">
-        <v>10</v>
-      </c>
+      <c r="D18" s="1">
+        <v>3932</v>
+      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="M18" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1154,18 +1195,21 @@
       <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1">
-        <v>10</v>
-      </c>
+      <c r="D19" s="1">
+        <v>3932</v>
+      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="M19" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1175,18 +1219,21 @@
       <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2">
+      <c r="D20" s="1">
+        <v>3936</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
         <v>5</v>
       </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="M20" s="1"/>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1196,18 +1243,21 @@
       <c r="C21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2">
+      <c r="D21" s="1">
+        <v>3936</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
         <v>5</v>
       </c>
-      <c r="F21" s="2">
-        <v>2</v>
-      </c>
-      <c r="M21" s="1"/>
+      <c r="G21" s="2">
+        <v>2</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1216,11 +1266,12 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="G22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1229,17 +1280,18 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="M23" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G23" s="1"/>
       <c r="N23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O23" s="1">
+      <c r="O23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P23" s="1">
         <v>0.625</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1248,17 +1300,18 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="M24" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G24" s="1"/>
       <c r="N24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P24" s="1">
         <v>0.313</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1267,17 +1320,18 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="M25" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G25" s="1"/>
       <c r="N25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P25" s="1">
         <v>0.156</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1287,18 +1341,19 @@
       <c r="C26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1">
         <v>5</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="M26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1308,15 +1363,16 @@
       <c r="C27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1">
         <v>5</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1326,15 +1382,18 @@
       <c r="C28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1">
-        <v>10</v>
-      </c>
+      <c r="D28" s="1">
+        <v>3921</v>
+      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1344,15 +1403,18 @@
       <c r="C29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1">
-        <v>10</v>
-      </c>
+      <c r="D29" s="1">
+        <v>3921</v>
+      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1362,15 +1424,18 @@
       <c r="C30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1">
-        <v>10</v>
-      </c>
+      <c r="D30" s="1">
+        <v>3933</v>
+      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1380,15 +1445,18 @@
       <c r="C31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1">
-        <v>10</v>
-      </c>
+      <c r="D31" s="1">
+        <v>3933</v>
+      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1398,15 +1466,18 @@
       <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2">
+      <c r="D32" s="1">
+        <v>3937</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2">
         <v>5</v>
       </c>
-      <c r="F32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1416,15 +1487,18 @@
       <c r="C33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2">
+      <c r="D33" s="1">
+        <v>3937</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2">
         <v>5</v>
       </c>
-      <c r="F33" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -1433,8 +1507,9 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -1443,8 +1518,9 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1453,8 +1529,9 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -1463,8 +1540,9 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1474,15 +1552,16 @@
       <c r="C38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1">
         <v>2.5</v>
       </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -1492,15 +1571,16 @@
       <c r="C39" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1">
         <v>2.5</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="1"/>
+      <c r="G39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -1510,15 +1590,18 @@
       <c r="C40" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1">
-        <v>10</v>
-      </c>
+      <c r="D40" s="1">
+        <v>3921</v>
+      </c>
+      <c r="E40" s="1"/>
       <c r="F40" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
@@ -1528,15 +1611,18 @@
       <c r="C41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1">
-        <v>10</v>
-      </c>
+      <c r="D41" s="1">
+        <v>3921</v>
+      </c>
+      <c r="E41" s="1"/>
       <c r="F41" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
@@ -1546,15 +1632,18 @@
       <c r="C42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1">
-        <v>10</v>
-      </c>
+      <c r="D42" s="1">
+        <v>3933</v>
+      </c>
+      <c r="E42" s="1"/>
       <c r="F42" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
@@ -1564,15 +1653,18 @@
       <c r="C43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1">
-        <v>10</v>
-      </c>
+      <c r="D43" s="1">
+        <v>3933</v>
+      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -1582,15 +1674,18 @@
       <c r="C44" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2">
+      <c r="D44" s="1">
+        <v>3937</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2">
         <v>5</v>
       </c>
-      <c r="F44" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -1600,15 +1695,18 @@
       <c r="C45" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2">
+      <c r="D45" s="1">
+        <v>3937</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2">
         <v>5</v>
       </c>
-      <c r="F45" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
@@ -1617,8 +1715,9 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -1627,8 +1726,9 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -1637,8 +1737,9 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>55</v>
       </c>
@@ -1647,8 +1748,9 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>56</v>
       </c>
@@ -1658,15 +1760,16 @@
       <c r="C50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1">
         <v>1.25</v>
       </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F50" s="1"/>
+      <c r="G50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
@@ -1676,15 +1779,16 @@
       <c r="C51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1">
         <v>1.25</v>
       </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F51" s="1"/>
+      <c r="G51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -1694,15 +1798,18 @@
       <c r="C52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1">
-        <v>10</v>
-      </c>
+      <c r="D52" s="1">
+        <v>3922</v>
+      </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>62</v>
       </c>
@@ -1712,15 +1819,18 @@
       <c r="C53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1">
-        <v>10</v>
-      </c>
+      <c r="D53" s="1">
+        <v>3922</v>
+      </c>
+      <c r="E53" s="1"/>
       <c r="F53" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>63</v>
       </c>
@@ -1730,15 +1840,18 @@
       <c r="C54" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1">
+      <c r="D54" s="2">
+        <v>3934</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1">
         <v>50</v>
       </c>
-      <c r="F54" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>64</v>
       </c>
@@ -1748,15 +1861,18 @@
       <c r="C55" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1">
+      <c r="D55" s="2">
+        <v>3934</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1">
         <v>50</v>
       </c>
-      <c r="F55" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1766,15 +1882,18 @@
       <c r="C56" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2">
+      <c r="D56" s="2">
+        <v>3938</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2">
         <v>5</v>
       </c>
-      <c r="F56" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>66</v>
       </c>
@@ -1784,15 +1903,18 @@
       <c r="C57" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2">
+      <c r="D57" s="2">
+        <v>3938</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2">
         <v>5</v>
       </c>
-      <c r="F57" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>67</v>
       </c>
@@ -1801,8 +1923,9 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
@@ -1811,8 +1934,9 @@
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>69</v>
       </c>
@@ -1821,8 +1945,9 @@
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>70</v>
       </c>
@@ -1831,8 +1956,9 @@
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
@@ -1842,15 +1968,16 @@
       <c r="C62" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1">
         <v>0.625</v>
       </c>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F62" s="1"/>
+      <c r="G62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
@@ -1860,15 +1987,16 @@
       <c r="C63" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1">
         <v>0.625</v>
       </c>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F63" s="1"/>
+      <c r="G63" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>75</v>
       </c>
@@ -1878,15 +2006,18 @@
       <c r="C64" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="2">
-        <v>10</v>
-      </c>
-      <c r="F64" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D64" s="2">
+        <v>3922</v>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="F64" s="2">
+        <v>10</v>
+      </c>
+      <c r="G64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
@@ -1896,15 +2027,18 @@
       <c r="C65" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D65" s="1"/>
-      <c r="E65" s="2">
-        <v>10</v>
-      </c>
-      <c r="F65" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D65" s="2">
+        <v>3922</v>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="F65" s="2">
+        <v>10</v>
+      </c>
+      <c r="G65" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>78</v>
       </c>
@@ -1914,15 +2048,18 @@
       <c r="C66" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D66" s="1"/>
-      <c r="E66" s="2">
+      <c r="D66" s="2">
+        <v>3934</v>
+      </c>
+      <c r="E66" s="1"/>
+      <c r="F66" s="2">
         <v>50</v>
       </c>
-      <c r="F66" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>79</v>
       </c>
@@ -1932,15 +2069,18 @@
       <c r="C67" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D67" s="1"/>
-      <c r="E67" s="2">
+      <c r="D67" s="2">
+        <v>3934</v>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="F67" s="2">
         <v>50</v>
       </c>
-      <c r="F67" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>80</v>
       </c>
@@ -1950,15 +2090,18 @@
       <c r="C68" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2">
+      <c r="D68" s="2">
+        <v>3938</v>
+      </c>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2">
         <v>5</v>
       </c>
-      <c r="F68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>81</v>
       </c>
@@ -1968,15 +2111,18 @@
       <c r="C69" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2">
+      <c r="D69" s="2">
+        <v>3938</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2">
         <v>5</v>
       </c>
-      <c r="F69" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>82</v>
       </c>
@@ -1985,8 +2131,9 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>83</v>
       </c>
@@ -1995,8 +2142,9 @@
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>84</v>
       </c>
@@ -2005,8 +2153,9 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>85</v>
       </c>
@@ -2015,8 +2164,9 @@
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>86</v>
       </c>
@@ -2026,15 +2176,16 @@
       <c r="C74" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="1"/>
+      <c r="E74" s="1">
         <v>0.313</v>
       </c>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F74" s="1"/>
+      <c r="G74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>87</v>
       </c>
@@ -2044,15 +2195,16 @@
       <c r="C75" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75" s="1"/>
+      <c r="E75" s="1">
         <v>0.313</v>
       </c>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F75" s="1"/>
+      <c r="G75" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>88</v>
       </c>
@@ -2062,15 +2214,18 @@
       <c r="C76" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="2">
-        <v>10</v>
-      </c>
-      <c r="F76" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D76" s="2">
+        <v>3923</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="F76" s="2">
+        <v>10</v>
+      </c>
+      <c r="G76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>89</v>
       </c>
@@ -2080,15 +2235,18 @@
       <c r="C77" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="2">
-        <v>10</v>
-      </c>
-      <c r="F77" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D77" s="2">
+        <v>3923</v>
+      </c>
+      <c r="E77" s="1"/>
+      <c r="F77" s="2">
+        <v>10</v>
+      </c>
+      <c r="G77" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>90</v>
       </c>
@@ -2098,15 +2256,18 @@
       <c r="C78" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D78" s="1"/>
-      <c r="E78" s="2">
-        <v>10</v>
-      </c>
-      <c r="F78" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D78" s="2">
+        <v>3935</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="2">
+        <v>10</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>91</v>
       </c>
@@ -2116,15 +2277,18 @@
       <c r="C79" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D79" s="1"/>
-      <c r="E79" s="2">
-        <v>10</v>
-      </c>
-      <c r="F79" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D79" s="2">
+        <v>3935</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="F79" s="2">
+        <v>10</v>
+      </c>
+      <c r="G79" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>92</v>
       </c>
@@ -2134,15 +2298,18 @@
       <c r="C80" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2">
+      <c r="D80" s="2">
+        <v>3939</v>
+      </c>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2">
         <v>5</v>
       </c>
-      <c r="F80" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>93</v>
       </c>
@@ -2152,15 +2319,18 @@
       <c r="C81" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2">
+      <c r="D81" s="2">
+        <v>3939</v>
+      </c>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2">
         <v>5</v>
       </c>
-      <c r="F81" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>94</v>
       </c>
@@ -2169,8 +2339,9 @@
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82" s="1"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>95</v>
       </c>
@@ -2179,8 +2350,9 @@
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83" s="1"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>96</v>
       </c>
@@ -2189,8 +2361,9 @@
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84" s="1"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>97</v>
       </c>
@@ -2199,8 +2372,9 @@
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85" s="1"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>98</v>
       </c>
@@ -2210,15 +2384,16 @@
       <c r="C86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86" s="1"/>
+      <c r="E86" s="1">
         <v>0.156</v>
       </c>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F86" s="1"/>
+      <c r="G86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>99</v>
       </c>
@@ -2228,15 +2403,16 @@
       <c r="C87" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87" s="1"/>
+      <c r="E87" s="1">
         <v>0.156</v>
       </c>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F87" s="1"/>
+      <c r="G87" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>100</v>
       </c>
@@ -2246,15 +2422,18 @@
       <c r="C88" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D88" s="1"/>
-      <c r="E88" s="2">
-        <v>10</v>
-      </c>
-      <c r="F88" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D88" s="2">
+        <v>3923</v>
+      </c>
+      <c r="E88" s="1"/>
+      <c r="F88" s="2">
+        <v>10</v>
+      </c>
+      <c r="G88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>101</v>
       </c>
@@ -2264,15 +2443,18 @@
       <c r="C89" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D89" s="1"/>
-      <c r="E89" s="2">
-        <v>10</v>
-      </c>
-      <c r="F89" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D89" s="2">
+        <v>3923</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="2">
+        <v>10</v>
+      </c>
+      <c r="G89" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>102</v>
       </c>
@@ -2282,15 +2464,18 @@
       <c r="C90" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D90" s="1"/>
-      <c r="E90" s="2">
-        <v>10</v>
-      </c>
-      <c r="F90" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D90" s="2">
+        <v>3935</v>
+      </c>
+      <c r="E90" s="1"/>
+      <c r="F90" s="2">
+        <v>10</v>
+      </c>
+      <c r="G90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>103</v>
       </c>
@@ -2300,15 +2485,18 @@
       <c r="C91" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D91" s="1"/>
-      <c r="E91" s="2">
-        <v>10</v>
-      </c>
-      <c r="F91" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D91" s="2">
+        <v>3935</v>
+      </c>
+      <c r="E91" s="1"/>
+      <c r="F91" s="2">
+        <v>10</v>
+      </c>
+      <c r="G91" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>104</v>
       </c>
@@ -2318,15 +2506,18 @@
       <c r="C92" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2">
+      <c r="D92" s="2">
+        <v>3939</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2">
         <v>5</v>
       </c>
-      <c r="F92" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>105</v>
       </c>
@@ -2336,15 +2527,18 @@
       <c r="C93" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2">
+      <c r="D93" s="2">
+        <v>3939</v>
+      </c>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2">
         <v>5</v>
       </c>
-      <c r="F93" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>106</v>
       </c>
@@ -2353,8 +2547,9 @@
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>107</v>
       </c>
@@ -2363,8 +2558,9 @@
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>108</v>
       </c>
@@ -2373,8 +2569,9 @@
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G96" s="1"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>109</v>
       </c>
@@ -2383,6 +2580,7 @@
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>